<commit_message>
joft mozdi borj 5 tamam shod
</commit_message>
<xml_diff>
--- a/پیمانکاری اکسل.xlsx
+++ b/پیمانکاری اکسل.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="فلاحتی" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="155">
   <si>
     <t>رسول فلاحتی</t>
   </si>
@@ -490,6 +490,15 @@
   </si>
   <si>
     <t>میناره اعلامی</t>
+  </si>
+  <si>
+    <t>374/1</t>
+  </si>
+  <si>
+    <t>نارنجی</t>
+  </si>
+  <si>
+    <t>کرم</t>
   </si>
 </sst>
 </file>
@@ -889,7 +898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -982,6 +991,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,6 +1031,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1052,24 +1085,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1381,14 +1396,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="2:7" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
@@ -3797,15 +3812,15 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
     </row>
     <row r="6" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -4636,11 +4651,11 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A2:H35"/>
+  <dimension ref="A2:H94"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="B2:G4"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.55000000000000004"/>
@@ -4656,14 +4671,14 @@
   <sheetData>
     <row r="2" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="3" spans="2:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="2:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="3" t="s">
@@ -5270,6 +5285,478 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5282,17 +5769,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="C3:H26"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView rightToLeft="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="9.140625" style="39"/>
+    <col min="6" max="6" width="8.42578125" style="39" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="39"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.6">
@@ -5304,202 +5796,218 @@
       <c r="H3" s="32"/>
     </row>
     <row r="4" spans="3:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="62"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
     </row>
     <row r="5" spans="3:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="64" t="s">
+      <c r="G5" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="65" t="s">
+      <c r="H5" s="38" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="C6" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="40">
+        <v>60</v>
+      </c>
+      <c r="G6" s="40">
+        <v>14030525</v>
+      </c>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="C7" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="40">
+        <v>60</v>
+      </c>
+      <c r="G7" s="40">
+        <v>14030525</v>
+      </c>
+      <c r="H7" s="40"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5531,15 +6039,15 @@
   <sheetData>
     <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="55"/>
     </row>
     <row r="5" spans="3:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
@@ -5733,15 +6241,15 @@
       </c>
     </row>
     <row r="14" spans="3:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="50"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
     </row>
     <row r="15" spans="3:9" ht="24" x14ac:dyDescent="0.25">
       <c r="C15" s="6"/>
@@ -5817,14 +6325,14 @@
   <sheetData>
     <row r="2" spans="3:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="3:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="61"/>
     </row>
     <row r="4" spans="3:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="12" t="s">
@@ -6964,14 +7472,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="56"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="64"/>
     </row>
     <row r="2" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -7201,14 +7709,14 @@
   <sheetData>
     <row r="4" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="3:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="59"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="67"/>
     </row>
     <row r="6" spans="3:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">

</xml_diff>

<commit_message>
Mahdi Haddadi RAFT !  akharin commit
</commit_message>
<xml_diff>
--- a/پیمانکاری اکسل.xlsx
+++ b/پیمانکاری اکسل.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="161">
   <si>
     <t>رسول فلاحتی</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>1403/06/09</t>
+  </si>
+  <si>
+    <t>1403/06/19</t>
   </si>
 </sst>
 </file>
@@ -4669,8 +4672,8 @@
   <dimension ref="A2:H94"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <pane ySplit="4" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.55000000000000004"/>
@@ -5342,11 +5345,21 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="1">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="1">
+        <v>180</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.55000000000000004">

</xml_diff>